<commit_message>
update: using moving window; both last peak
</commit_message>
<xml_diff>
--- a/standalong.xlsx
+++ b/standalong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natong\Desktop\RFID-UI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC20682E-A209-42B1-ABF8-5E436957A22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD92764-40D1-480E-AFFB-173325A77323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="16960" xr2:uid="{DEFF84B5-F738-4BD0-AF6B-FE902AB1182A}"/>
   </bookViews>
@@ -164,21 +164,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -503,12 +501,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.7265625" style="4"/>
-    <col min="5" max="5" width="19" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="5"/>
-    <col min="7" max="7" width="31" style="5" customWidth="1"/>
-    <col min="8" max="8" width="130.54296875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="4"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="4"/>
+    <col min="7" max="7" width="31" style="4" customWidth="1"/>
+    <col min="8" max="8" width="130.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="5:8" x14ac:dyDescent="0.35">
@@ -526,21 +522,21 @@
       </c>
     </row>
     <row r="5" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>139.99</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>69.989999999999995</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -548,10 +544,10 @@
       </c>
     </row>
     <row r="7" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>250</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -559,55 +555,55 @@
       </c>
     </row>
     <row r="8" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>1905</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f>272*2</f>
         <v>544</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>9.99</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>9.99</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -615,15 +611,15 @@
       <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="5:8" x14ac:dyDescent="0.35">
-      <c r="E14" s="4" t="s">
+      <c r="E14" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f>SUM(F5:F13)</f>
         <v>2928.9599999999996</v>
       </c>

</xml_diff>